<commit_message>
Working race and contracts
</commit_message>
<xml_diff>
--- a/wrestleverse_companies.xlsx
+++ b/wrestleverse_companies.xlsx
@@ -141,49 +141,47 @@
     <t>HOF</t>
   </si>
   <si>
-    <t>Clayton wrestling</t>
-  </si>
-  <si>
-    <t>Cw</t>
-  </si>
-  <si>
-    <t>www.claytonwrestling.com</t>
+    <t>Ultimate Fight Zone Association (UFZA)</t>
+  </si>
+  <si>
+    <t>UFZA</t>
+  </si>
+  <si>
+    <t>www.ultimatefightzoneassociation(ufza).c</t>
   </si>
   <si>
     <t>1666-01-01</t>
   </si>
   <si>
-    <t>claytonwrestling.jpg</t>
-  </si>
-  <si>
-    <t>claytonwrestlingBD.jpg</t>
-  </si>
-  <si>
-    <t>claytonwrestlingBanner.jpg</t>
+    <t>ultimatefightzoneassociation(ufza).</t>
+  </si>
+  <si>
+    <t>ultimatefightzoneassociation(ufza)B</t>
+  </si>
+  <si>
+    <t>ultimatefightzoneassociation(u</t>
   </si>
   <si>
     <t>Bio</t>
   </si>
   <si>
-    <t>Name: Clayton Wrestling 
-Description: Clayton Wrestling is a professional wrestling company that prides itself on its cutting-edge use of artificial intelligence in their matches and storylines. The company is considered medium in size, but has a dedicated fan base that appreciates their innovative approach to wrestling. 
-Motto: "Where AI meets the ring"
-Founder: Clayton Anderson 
-CEO: Ashley Clayton 
-Location: Based in Silicon Valley, California 
-Established: 2015 
-Roster: Clayton Wrestling boasts a diverse and talented roster of wrestlers from around the world. From high-flying aerial artists to technical submission specialists, there is something for every wrestling fan to enjoy at Clayton Wrestling. 
-Championships: The company features a range of championships, including the Clayton Heavyweight Championship, the Clayton Tag Team Championship, and the Clayton Women's Championship. 
-Events: Clayton Wrestling holds live events throughout the year, featuring unique match stipulations and exciting storylines driven by AI technology. Fans can expect thrilling action and unexpected twists at every show. 
-Fan Interaction: Clayton Wrestling values its fans and prides itself on its interactive approach to fan engagement. From meet and greets with the wrestlers to behind-the-scenes access, the company goes above and beyond to connect with its audience. 
-Partnerships: Clayton Wrestling has established partnerships with leading tech companies, allowing them to stay at the forefront of AI innovation in the wrestling world. These partnerships have helped the company to push the boundaries of what is possible in professional wrestling. 
-Overall, Clayton Wrestling is a forward-thinking and exciting company that offers a unique and engaging wrestling experience for fans. With a focus on AI technology and a commitment to innovation, Clayton Wrestling is not your average wrestling company.</t>
+    <t>Name: Ultimate Fight Zone Association (UFZA)
+Founder: John Smith
+Established in: 2005
+Location: Orlando, Florida
+Size: Medium
+About UFZA:
+Ultimate Fight Zone Association (UFZA) is a professional wrestling company based in Orlando, Florida. Established in 2005 by founder John Smith, UFZA has quickly become known for its intense and action-packed wrestling matches. The company is considered medium in size and has a dedicated fan base that spans across the United States.
+UFZA has a roster of talented wrestlers, including both seasoned veterans and up-and-coming stars. The company prides itself on providing top-notch entertainment for its fans, with high-energy matches and captivating storylines that keep audiences on the edge of their seats.
+UFZA hosts live events in various cities across the country, drawing in crowds of enthusiastic fans who come to witness the thrilling action firsthand. The company also produces a weekly television show that showcases the best matches and moments from their live events.
+In addition to live events and television programming, UFZA offers merchandise featuring their logo and the likenesses of their top wrestlers. Fans can purchase t-shirts, hats, posters, and more to show their support for their favorite UFZA stars.
+Ultimate Fight Zone Association is committed to providing a platform for talented wrestlers to showcase their skills and entertain fans with their athleticism and charisma. With a focus on high-quality wrestling and engaging storytelling, UFZA continues to grow its fan base and solidify its reputation as a premier professional wrestling company.</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>A very pro "AI" wrestling company that takes AI very seriously in their wrestling.</t>
+    <t>a sports wrestling company</t>
   </si>
   <si>
     <t>Medium</t>
@@ -677,7 +675,7 @@
     </row>
     <row r="2" spans="1:41">
       <c r="A2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -713,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -728,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="R2">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -814,7 +812,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Adding flags to excel to set up image generation
</commit_message>
<xml_diff>
--- a/wrestleverse_companies.xlsx
+++ b/wrestleverse_companies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>UID</t>
   </si>
@@ -141,47 +141,48 @@
     <t>HOF</t>
   </si>
   <si>
-    <t>Ultimate Fight Zone Association (UFZA)</t>
-  </si>
-  <si>
-    <t>UFZA</t>
-  </si>
-  <si>
-    <t>www.ultimatefightzoneassociation(ufza).c</t>
+    <t>testee</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>www.testee.com</t>
   </si>
   <si>
     <t>1666-01-01</t>
   </si>
   <si>
-    <t>ultimatefightzoneassociation(ufza).</t>
-  </si>
-  <si>
-    <t>ultimatefightzoneassociation(ufza)B</t>
-  </si>
-  <si>
-    <t>ultimatefightzoneassociation(u</t>
+    <t>testee.jpg</t>
+  </si>
+  <si>
+    <t>testeeBD.jpg</t>
+  </si>
+  <si>
+    <t>testeeBanner.jpg</t>
   </si>
   <si>
     <t>Bio</t>
   </si>
   <si>
-    <t>Name: Ultimate Fight Zone Association (UFZA)
-Founder: John Smith
-Established in: 2005
-Location: Orlando, Florida
-Size: Medium
-About UFZA:
-Ultimate Fight Zone Association (UFZA) is a professional wrestling company based in Orlando, Florida. Established in 2005 by founder John Smith, UFZA has quickly become known for its intense and action-packed wrestling matches. The company is considered medium in size and has a dedicated fan base that spans across the United States.
-UFZA has a roster of talented wrestlers, including both seasoned veterans and up-and-coming stars. The company prides itself on providing top-notch entertainment for its fans, with high-energy matches and captivating storylines that keep audiences on the edge of their seats.
-UFZA hosts live events in various cities across the country, drawing in crowds of enthusiastic fans who come to witness the thrilling action firsthand. The company also produces a weekly television show that showcases the best matches and moments from their live events.
-In addition to live events and television programming, UFZA offers merchandise featuring their logo and the likenesses of their top wrestlers. Fans can purchase t-shirts, hats, posters, and more to show their support for their favorite UFZA stars.
-Ultimate Fight Zone Association is committed to providing a platform for talented wrestlers to showcase their skills and entertain fans with their athleticism and charisma. With a focus on high-quality wrestling and engaging storytelling, UFZA continues to grow its fan base and solidify its reputation as a premier professional wrestling company.</t>
+    <t>Name: Testee Wrestling
+Description: Testee Wrestling is a professional wrestling company that focuses on testing the skills and abilities of its wrestlers in the ring. The company is medium in size and operates across various regions, hosting events and shows throughout the year.
+History: Testee Wrestling was founded by a group of wrestling enthusiasts who wanted to create a platform where aspiring wrestlers could showcase their talent and improve their skills. The company started small but quickly gained popularity for its unique approach to wrestling contests.
+Location: Testee Wrestling is headquartered in a bustling city, but it hosts events in various locations across the country. The company has a dedicated team of staff members who work tirelessly to ensure that each show is a success.
+Roster: The Testee Wrestling roster consists of a diverse group of talented wrestlers who come from various backgrounds and have different wrestling styles. From high-flying acrobats to powerhouse brawlers, the roster is designed to challenge each wrestler and push them to their limits.
+Events: Testee Wrestling hosts regular events throughout the year, including live shows, pay-per-view events, and special tournaments. Each event is carefully curated to test the skills and abilities of the wrestlers, with intense matches and exciting storylines that keep fans on the edge of their seats.
+Training: Testee Wrestling also offers training programs for aspiring wrestlers who want to improve their craft and potentially join the roster. The company has a state-of-the-art training facility where wrestlers can hone their skills under the guidance of experienced coaches and trainers.
+Fanbase: Testee Wrestling has a dedicated fanbase of wrestling enthusiasts who appreciate the company's focus on testing and showcasing talent in the ring. Fans eagerly await each event and cheer on their favorite wrestlers as they compete for glory and championships.
+Overall, Testee Wrestling is a unique and dynamic professional wrestling company that offers a platform for aspiring wrestlers to test their skills and abilities. With a talented roster, exciting events, and a passionate fanbase, Testee Wrestling is poised to continue growing and making a name for itself in the world of professional wrestling.</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>a sports wrestling company</t>
+    <t>image_generated</t>
+  </si>
+  <si>
+    <t>a testing company</t>
   </si>
   <si>
     <t>Medium</t>
@@ -675,7 +676,7 @@
     </row>
     <row r="2" spans="1:41">
       <c r="A2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -711,7 +712,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -726,7 +727,7 @@
         <v>10</v>
       </c>
       <c r="R2">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -812,7 +813,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
@@ -825,13 +826,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -841,16 +842,40 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a stable version trying to fix excel
</commit_message>
<xml_diff>
--- a/wrestleverse_companies.xlsx
+++ b/wrestleverse_companies.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t>UID</t>
   </si>
@@ -141,39 +141,39 @@
     <t>HOF</t>
   </si>
   <si>
-    <t>testee</t>
+    <t>thecomp</t>
   </si>
   <si>
     <t>t</t>
   </si>
   <si>
-    <t>www.testee.com</t>
+    <t>www.thecomp.com</t>
   </si>
   <si>
     <t>1666-01-01</t>
   </si>
   <si>
-    <t>testee.jpg</t>
-  </si>
-  <si>
-    <t>testeeBD.jpg</t>
-  </si>
-  <si>
-    <t>testeeBanner.jpg</t>
+    <t>thecomp.jpg</t>
+  </si>
+  <si>
+    <t>thecompBD.jpg</t>
+  </si>
+  <si>
+    <t>thecompBanner.jpg</t>
   </si>
   <si>
     <t>Bio</t>
   </si>
   <si>
-    <t>Name: Testee Wrestling
-Description: Testee Wrestling is a professional wrestling company that focuses on testing the skills and abilities of its wrestlers in the ring. The company is medium in size and operates across various regions, hosting events and shows throughout the year.
-History: Testee Wrestling was founded by a group of wrestling enthusiasts who wanted to create a platform where aspiring wrestlers could showcase their talent and improve their skills. The company started small but quickly gained popularity for its unique approach to wrestling contests.
-Location: Testee Wrestling is headquartered in a bustling city, but it hosts events in various locations across the country. The company has a dedicated team of staff members who work tirelessly to ensure that each show is a success.
-Roster: The Testee Wrestling roster consists of a diverse group of talented wrestlers who come from various backgrounds and have different wrestling styles. From high-flying acrobats to powerhouse brawlers, the roster is designed to challenge each wrestler and push them to their limits.
-Events: Testee Wrestling hosts regular events throughout the year, including live shows, pay-per-view events, and special tournaments. Each event is carefully curated to test the skills and abilities of the wrestlers, with intense matches and exciting storylines that keep fans on the edge of their seats.
-Training: Testee Wrestling also offers training programs for aspiring wrestlers who want to improve their craft and potentially join the roster. The company has a state-of-the-art training facility where wrestlers can hone their skills under the guidance of experienced coaches and trainers.
-Fanbase: Testee Wrestling has a dedicated fanbase of wrestling enthusiasts who appreciate the company's focus on testing and showcasing talent in the ring. Fans eagerly await each event and cheer on their favorite wrestlers as they compete for glory and championships.
-Overall, Testee Wrestling is a unique and dynamic professional wrestling company that offers a platform for aspiring wrestlers to test their skills and abilities. With a talented roster, exciting events, and a passionate fanbase, Testee Wrestling is poised to continue growing and making a name for itself in the world of professional wrestling.</t>
+    <t>Name: thecomp
+Promotion Type: Professional Wrestling Company
+Size: Medium
+Location: TBD
+Description:
+thecomp is a professional wrestling company that prides itself on providing high-quality, entertaining wrestling matches for fans all over the world. As a test company, thecomp is constantly striving to push the boundaries of traditional wrestling and create new and innovative content for its audience.
+Founded by a group of wrestling enthusiasts, thecomp has quickly gained a reputation for showcasing some of the best talent in the industry. With a roster of skilled and passionate wrestlers, thecomp offers a diverse range of styles and personalities, ensuring that there is something for every fan to enjoy.
+In addition to its in-ring action, thecomp also focuses on creating engaging storylines and rivalries that captivate audiences and keep them coming back for more. The company also places a strong emphasis on fan interaction, regularly hosting meet-and-greet events and Q&amp;A sessions with its wrestlers.
+With a dedicated and hardworking team behind the scenes, thecomp is committed to providing a professional and entertaining product that fans can be proud to support. Whether you're a longtime wrestling fan or new to the sport, thecomp has something for everyone to enjoy. Stay tuned for upcoming events and shows from thecomp!</t>
   </si>
   <si>
     <t>Description</t>
@@ -182,10 +182,16 @@
     <t>image_generated</t>
   </si>
   <si>
-    <t>a testing company</t>
+    <t>logo_description</t>
+  </si>
+  <si>
+    <t>a test company</t>
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>The logo for 'thecomp' may feature a bold, modern font in black and white with a stylized wrestling ring silhouette in the background, symbolizing strength and competition.</t>
   </si>
 </sst>
 </file>
@@ -676,7 +682,7 @@
     </row>
     <row r="2" spans="1:41">
       <c r="A2">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -712,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -727,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="R2">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -813,7 +819,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
@@ -826,13 +832,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -854,16 +860,19 @@
       <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -876,6 +885,9 @@
       </c>
       <c r="G2" t="b">
         <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think working version, company excel overwrites
</commit_message>
<xml_diff>
--- a/wrestleverse_companies.xlsx
+++ b/wrestleverse_companies.xlsx
@@ -141,39 +141,45 @@
     <t>HOF</t>
   </si>
   <si>
-    <t>thecomp</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>www.thecomp.com</t>
+    <t>"Game On Wrestling Federation"</t>
+  </si>
+  <si>
+    <t>OWF</t>
+  </si>
+  <si>
+    <t>www."gameonwrestlingfederation".com</t>
   </si>
   <si>
     <t>1666-01-01</t>
   </si>
   <si>
-    <t>thecomp.jpg</t>
-  </si>
-  <si>
-    <t>thecompBD.jpg</t>
-  </si>
-  <si>
-    <t>thecompBanner.jpg</t>
+    <t>"gameonwrestlingfederation".jpg</t>
+  </si>
+  <si>
+    <t>"gameonwrestlingfederation"BD.jpg</t>
+  </si>
+  <si>
+    <t>"gameonwrestlingfederation"Ban</t>
   </si>
   <si>
     <t>Bio</t>
   </si>
   <si>
-    <t>Name: thecomp
-Promotion Type: Professional Wrestling Company
+    <t>Name: Game On Wrestling Federation
+Location: TBD
 Size: Medium
-Location: TBD
 Description:
-thecomp is a professional wrestling company that prides itself on providing high-quality, entertaining wrestling matches for fans all over the world. As a test company, thecomp is constantly striving to push the boundaries of traditional wrestling and create new and innovative content for its audience.
-Founded by a group of wrestling enthusiasts, thecomp has quickly gained a reputation for showcasing some of the best talent in the industry. With a roster of skilled and passionate wrestlers, thecomp offers a diverse range of styles and personalities, ensuring that there is something for every fan to enjoy.
-In addition to its in-ring action, thecomp also focuses on creating engaging storylines and rivalries that captivate audiences and keep them coming back for more. The company also places a strong emphasis on fan interaction, regularly hosting meet-and-greet events and Q&amp;A sessions with its wrestlers.
-With a dedicated and hardworking team behind the scenes, thecomp is committed to providing a professional and entertaining product that fans can be proud to support. Whether you're a longtime wrestling fan or new to the sport, thecomp has something for everyone to enjoy. Stay tuned for upcoming events and shows from thecomp!</t>
+Game On Wrestling Federation is a unique and innovative professional wrestling company that combines the thrill and excitement of a gameshow with the physicality and drama of professional wrestling. With a medium-sized roster of talented and charismatic wrestlers, GOWF offers a fresh and exciting take on sports entertainment.
+Theme:
+The theme of GOWF is all about competition and entertainment. Each wrestling event is designed like a gameshow, with different segments and matches that challenge the competitors in various ways. From trivia rounds to physical challenges, the wrestlers must showcase their skills not only in the ring but also in a range of different game formats.
+Roster:
+The roster of GOWF is diverse and eclectic, featuring a mix of seasoned veterans and up-and-coming talent. Wrestlers in the company are known for their athleticism, charisma, and willingness to take risks in order to entertain the audience. The roster includes a mix of traditional wrestlers, high-flying acrobats, and comedic characters, all of whom bring something unique to the ring.
+Championships:
+GOWF features a range of championships that are hotly contested by the wrestlers on the roster. Titles include the Game On Championship, which is the top prize in the company and is defended in high-stakes matches that combine in-ring action with gameshow-style challenges. Other titles include the Tag Team Championship, the Women's Championship, and the Hardcore Championship.
+Events:
+GOWF hosts regular wrestling events that are broadcast on television and live-streamed online for fans around the world to enjoy. Each event features a mix of traditional wrestling matches and gameshow-style challenges, with surprises and twists that keep the audience on the edge of their seats. From one-on-one grudge matches to multi-man spectacles, GOWF events are always full of excitement and drama.
+Mission:
+The mission of GOWF is to provide fans with a fresh and engaging alternative to traditional professional wrestling. By combining the excitement of a gameshow with the physicality of wrestling, GOWF offers a unique entertainment experience that appeals to a wide range of viewers. The company is dedicated to pushing the boundaries of what is possible in the world of sports entertainment and creating memorable moments that will keep fans coming back for more.</t>
   </si>
   <si>
     <t>Description</t>
@@ -185,13 +191,13 @@
     <t>logo_description</t>
   </si>
   <si>
-    <t>a test company</t>
+    <t>a gameshow themed wrestling company</t>
   </si>
   <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>The logo for 'thecomp' may feature a bold, modern font in black and white with a stylized wrestling ring silhouette in the background, symbolizing strength and competition.</t>
+    <t>The logo for Game On Wrestling Federation would feature bold, vibrant colors, retro arcade fonts, and a mix of wrestling and game show symbols such as wrestling ring ropes intertwined with game controllers, dice, and a spotlight shining down on a wrestling championship belt.</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
     </row>
     <row r="2" spans="1:41">
       <c r="A2">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -718,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="M2">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -733,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="R2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -819,7 +825,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Working images for wrestlers and companies
</commit_message>
<xml_diff>
--- a/wrestleverse_companies.xlsx
+++ b/wrestleverse_companies.xlsx
@@ -669,21 +669,21 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Athletic Fury Wrestling Co.</t>
+          <t>Bubba</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AFWC</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>www.athleticfurywrestlingco..com</t>
+          <t>www.bubba.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -704,24 +704,24 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco..jpg</t>
+          <t>bubba.jpg</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco.BD.jpg</t>
+          <t>bubbaBD.jpg</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco.Banner</t>
+          <t>bubbaBN.jpg</t>
         </is>
       </c>
       <c r="L2" t="n">
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="R2" t="n">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
@@ -836,18 +836,29 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Name: Athletic Fury Wrestling Co.
-Location: United States
-Established: 2010
+          <t>Name: Bubba Wrestling Federation
+Location: Bubba City, USA
+Founded: 2020
 Size: Medium
-Athletic Fury Wrestling Co. is a professional wrestling company that specializes in sports-themed wrestling events. Founded in 2010, the company has quickly made a name for itself in the wrestling world by offering high-energy, action-packed matches that cater to both hardcore wrestling fans and casual sports enthusiasts.
-With a medium-sized roster of talented wrestlers from around the world, Athletic Fury Wrestling Co. puts on shows that feature a mix of traditional wrestling styles, high-flying acrobatics, and hard-hitting brawls. The company prides itself on showcasing the athleticism and skill of its performers, while also providing entertaining storylines and feuds that keep fans on the edge of their seats.
-Athletic Fury Wrestling Co. is known for its dedication to providing a family-friendly atmosphere at its events, ensuring that fans of all ages can enjoy the action without worry. The company also places a strong emphasis on community outreach, regularly hosting charity events and fundraisers to give back to the local areas where it operates.
-As a medium-sized wrestling company, Athletic Fury Wrestling Co. has carved out a niche in the industry by focusing on quality over quantity. With a loyal fanbase and a reputation for delivering top-notch entertainment, the company continues to grow and expand its reach, attracting new fans and talent along the way.</t>
+Overview:
+Bubba Wrestling Federation (BWF) is a new professional wrestling company that is making waves in the industry. Founded in 2020, BWF has quickly gained a reputation for its exciting matches, talented roster, and innovative storytelling.
+Roster:
+BWF boasts a diverse and talented roster of wrestlers from all corners of the globe. From high-flying cruiserweights to powerhouse heavyweights, BWF has something for every wrestling fan. Some of the top stars of BWF include "The Phenom" Alex Black, "The Queen of Chaos" Ruby Reign, and "The Canadian Crusher" Jake Maverick.
+Show Format:
+BWF puts on weekly television shows that feature a mix of singles matches, tag team matches, and special events. The company also hosts monthly pay-per-view events that showcase the best of BWF's roster in high-stakes matches and intense rivalries.
+Titles:
+BWF currently has four championship titles that are contested for on a regular basis. These titles include the BWF World Heavyweight Championship, the BWF Women's Championship, the BWF Tag Team Championships, and the BWF Cruiserweight Championship. These titles are highly coveted and fiercely contested by the talented wrestlers of BWF.
+Storylines:
+BWF is known for its engaging and compelling storytelling. Whether it's a bitter rivalry between two wrestlers or a dramatic betrayal within a tag team, BWF's storylines keep fans on the edge of their seats. The creative team at BWF works tirelessly to craft entertaining and unpredictable storylines that keep fans coming back for more.
+Production:
+BWF spares no expense when it comes to the production of its shows. The company's state-of-the-art production team ensures that each event is visually stunning and professionally executed. From pyrotechnics to elaborate entrances, BWF's production values are top-notch and on par with some of the biggest wrestling companies in the world.
+Community Involvement:
+BWF is committed to giving back to the community and regularly partners with local charities and organizations to make a positive impact. Whether it's hosting fundraising events or volunteering at local schools, BWF is dedicated to using its platform to support those in need.
+Overall, BWF is a dynamic and exciting wrestling company that is quickly making a name for itself in the industry. With its talented roster, engaging storylines, and high-quality production values, BWF is a must-watch for any wrestling fan.</t>
         </is>
       </c>
     </row>
@@ -915,12 +926,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Athletic Fury Wrestling Co.</t>
+          <t>Bubba</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a sports themed wrestling company</t>
+          <t>A new wrestling company</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -930,17 +941,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco..jpg</t>
+          <t>bubba.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco.BD.jpg</t>
+          <t>bubbaBD.jpg</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>athleticfurywrestlingco.Banner</t>
+          <t>bubbaBanner.jpg</t>
         </is>
       </c>
       <c r="G2" t="b">
@@ -948,7 +959,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>The logo for Athletic Fury Wrestling Co. might feature bold, dynamic text in a fiery red and black color scheme, with silhouettes of muscular wrestlers in action poses surrounding a center image of crossed wrestling ropes.</t>
+          <t>The logo for 'Bubba' would likely feature bold and modern font in red and black color scheme, with a silhouette of a wrestler throwing a high-flying move.</t>
         </is>
       </c>
     </row>

</xml_diff>